<commit_message>
Post project, final push of code. Compilable again
</commit_message>
<xml_diff>
--- a/Inventory/Exports/ExportedInventory.xlsx
+++ b/Inventory/Exports/ExportedInventory.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="256">
   <si>
     <t>NAME</t>
   </si>
@@ -604,28 +604,37 @@
     <t>Super Mario Bros.  - GB</t>
   </si>
   <si>
-    <t>Uncharted 3: Drakes Deception  - PS3</t>
-  </si>
-  <si>
-    <t>Assassins Creed III  - PS3</t>
-  </si>
-  <si>
-    <t>Assassins Creed II  - PS3</t>
-  </si>
-  <si>
-    <t>Assassins Creed  - X360</t>
-  </si>
-  <si>
-    <t>Assassins Creed III  - X360</t>
-  </si>
-  <si>
-    <t>Assassins Creed II  - X360</t>
-  </si>
-  <si>
-    <t>Donkey Kong Country 2: Diddys Kong Quest  - SNES</t>
-  </si>
-  <si>
-    <t>Kirbys Dream Land  - GB</t>
+    <t>Super Sonic - Genesis</t>
+  </si>
+  <si>
+    <t>Super Monkey Ball - Genesis</t>
+  </si>
+  <si>
+    <t>Crazy Taxi - Genesis</t>
+  </si>
+  <si>
+    <t>Crazy Taxi 2- Genesis</t>
+  </si>
+  <si>
+    <t>Sonic Racing</t>
+  </si>
+  <si>
+    <t>Persona 5 - PS5</t>
+  </si>
+  <si>
+    <t>Persona 4 - PS5</t>
+  </si>
+  <si>
+    <t>Gundum Revolt - PS5</t>
+  </si>
+  <si>
+    <t>Barbie Magical Fashion</t>
+  </si>
+  <si>
+    <t>Barbie: Explorer</t>
+  </si>
+  <si>
+    <t>1234</t>
   </si>
   <si>
     <t>nan</t>
@@ -688,6 +697,15 @@
     <t>WiiU.jfif</t>
   </si>
   <si>
+    <t>sega.pdf</t>
+  </si>
+  <si>
+    <t>Gundum.pdf</t>
+  </si>
+  <si>
+    <t>Barbie.pdf</t>
+  </si>
+  <si>
     <t>Nintendo</t>
   </si>
   <si>
@@ -752,6 +770,18 @@
   </si>
   <si>
     <t>RedOctane</t>
+  </si>
+  <si>
+    <t>Sega Genesis</t>
+  </si>
+  <si>
+    <t>PS5</t>
+  </si>
+  <si>
+    <t>GBC</t>
+  </si>
+  <si>
+    <t>PS1</t>
   </si>
 </sst>
 </file>
@@ -1109,7 +1139,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F199"/>
+  <dimension ref="A1:F201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1140,19 +1170,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D2">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E2">
         <v>19.99</v>
       </c>
       <c r="F2" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1160,19 +1190,19 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C3" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D3">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3">
         <v>39.99</v>
       </c>
       <c r="F3" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1180,10 +1210,10 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C4" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D4">
         <v>33</v>
@@ -1192,7 +1222,7 @@
         <v>39.99</v>
       </c>
       <c r="F4" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1200,10 +1230,10 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C5" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D5">
         <v>31</v>
@@ -1212,7 +1242,7 @@
         <v>19.99</v>
       </c>
       <c r="F5" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1220,19 +1250,19 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C6" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6">
         <v>19.99</v>
       </c>
       <c r="F6" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1240,10 +1270,10 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C7" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D7">
         <v>30</v>
@@ -1252,7 +1282,7 @@
         <v>39.99</v>
       </c>
       <c r="F7" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1260,19 +1290,19 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C8" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D8">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E8">
         <v>39.99</v>
       </c>
       <c r="F8" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1280,10 +1310,10 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C9" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D9">
         <v>28</v>
@@ -1292,7 +1322,7 @@
         <v>39.99</v>
       </c>
       <c r="F9" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1300,10 +1330,10 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C10" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D10">
         <v>28</v>
@@ -1312,7 +1342,7 @@
         <v>19.99</v>
       </c>
       <c r="F10" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1320,10 +1350,10 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C11" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D11">
         <v>24</v>
@@ -1332,7 +1362,7 @@
         <v>39.99</v>
       </c>
       <c r="F11" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1340,10 +1370,10 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C12" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D12">
         <v>23</v>
@@ -1352,7 +1382,7 @@
         <v>39.99</v>
       </c>
       <c r="F12" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1360,10 +1390,10 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C13" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D13">
         <v>23</v>
@@ -1372,7 +1402,7 @@
         <v>19.99</v>
       </c>
       <c r="F13" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1380,10 +1410,10 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C14" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D14">
         <v>22</v>
@@ -1392,7 +1422,7 @@
         <v>39.99</v>
       </c>
       <c r="F14" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1400,10 +1430,10 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C15" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D15">
         <v>22</v>
@@ -1412,7 +1442,7 @@
         <v>39.99</v>
       </c>
       <c r="F15" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1420,10 +1450,10 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C16" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D16">
         <v>21</v>
@@ -1432,7 +1462,7 @@
         <v>39.99</v>
       </c>
       <c r="F16" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1440,19 +1470,19 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C17" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D17">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E17">
         <v>49.99</v>
       </c>
       <c r="F17" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1460,10 +1490,10 @@
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C18" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D18">
         <v>20</v>
@@ -1472,7 +1502,7 @@
         <v>39.99</v>
       </c>
       <c r="F18" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1480,10 +1510,10 @@
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C19" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D19">
         <v>20</v>
@@ -1492,7 +1522,7 @@
         <v>19.99</v>
       </c>
       <c r="F19" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1500,10 +1530,10 @@
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C20" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D20">
         <v>20</v>
@@ -1512,7 +1542,7 @@
         <v>39.99</v>
       </c>
       <c r="F20" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1520,10 +1550,10 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C21" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D21">
         <v>18</v>
@@ -1532,7 +1562,7 @@
         <v>39.99</v>
       </c>
       <c r="F21" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1540,10 +1570,10 @@
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C22" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D22">
         <v>18</v>
@@ -1552,7 +1582,7 @@
         <v>19.99</v>
       </c>
       <c r="F22" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1560,10 +1590,10 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C23" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D23">
         <v>17</v>
@@ -1572,7 +1602,7 @@
         <v>19.99</v>
       </c>
       <c r="F23" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1580,10 +1610,10 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C24" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D24">
         <v>16</v>
@@ -1592,7 +1622,7 @@
         <v>49.99</v>
       </c>
       <c r="F24" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1600,10 +1630,10 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C25" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D25">
         <v>16</v>
@@ -1612,7 +1642,7 @@
         <v>39.99</v>
       </c>
       <c r="F25" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1620,10 +1650,10 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C26" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D26">
         <v>15</v>
@@ -1632,7 +1662,7 @@
         <v>39.99</v>
       </c>
       <c r="F26" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1640,10 +1670,10 @@
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C27" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D27">
         <v>15</v>
@@ -1652,7 +1682,7 @@
         <v>39.99</v>
       </c>
       <c r="F27" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1660,10 +1690,10 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C28" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D28">
         <v>15</v>
@@ -1672,7 +1702,7 @@
         <v>39.99</v>
       </c>
       <c r="F28" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1680,10 +1710,10 @@
         <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C29" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D29">
         <v>14</v>
@@ -1692,7 +1722,7 @@
         <v>39.99</v>
       </c>
       <c r="F29" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1700,10 +1730,10 @@
         <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C30" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D30">
         <v>14</v>
@@ -1712,7 +1742,7 @@
         <v>49.99</v>
       </c>
       <c r="F30" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1720,10 +1750,10 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C31" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D31">
         <v>14</v>
@@ -1732,7 +1762,7 @@
         <v>19.99</v>
       </c>
       <c r="F31" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1740,10 +1770,10 @@
         <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C32" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D32">
         <v>14</v>
@@ -1752,7 +1782,7 @@
         <v>39.99</v>
       </c>
       <c r="F32" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1760,10 +1790,10 @@
         <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C33" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D33">
         <v>14</v>
@@ -1772,7 +1802,7 @@
         <v>49.99</v>
       </c>
       <c r="F33" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1780,10 +1810,10 @@
         <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C34" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D34">
         <v>14</v>
@@ -1792,7 +1822,7 @@
         <v>49.99</v>
       </c>
       <c r="F34" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1800,10 +1830,10 @@
         <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C35" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D35">
         <v>14</v>
@@ -1812,7 +1842,7 @@
         <v>49.99</v>
       </c>
       <c r="F35" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1820,10 +1850,10 @@
         <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C36" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D36">
         <v>13</v>
@@ -1832,7 +1862,7 @@
         <v>49.99</v>
       </c>
       <c r="F36" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1840,10 +1870,10 @@
         <v>41</v>
       </c>
       <c r="B37" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C37" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D37">
         <v>13</v>
@@ -1852,7 +1882,7 @@
         <v>39.99</v>
       </c>
       <c r="F37" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1860,10 +1890,10 @@
         <v>42</v>
       </c>
       <c r="B38" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C38" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D38">
         <v>13</v>
@@ -1872,7 +1902,7 @@
         <v>49.99</v>
       </c>
       <c r="F38" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1880,10 +1910,10 @@
         <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C39" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D39">
         <v>13</v>
@@ -1892,7 +1922,7 @@
         <v>39.99</v>
       </c>
       <c r="F39" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1900,10 +1930,10 @@
         <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C40" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D40">
         <v>13</v>
@@ -1912,7 +1942,7 @@
         <v>39.99</v>
       </c>
       <c r="F40" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1920,10 +1950,10 @@
         <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C41" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D41">
         <v>12</v>
@@ -1932,7 +1962,7 @@
         <v>39.99</v>
       </c>
       <c r="F41" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1940,10 +1970,10 @@
         <v>46</v>
       </c>
       <c r="B42" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C42" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D42">
         <v>12</v>
@@ -1952,7 +1982,7 @@
         <v>39.99</v>
       </c>
       <c r="F42" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1960,10 +1990,10 @@
         <v>47</v>
       </c>
       <c r="B43" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C43" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D43">
         <v>12</v>
@@ -1972,7 +2002,7 @@
         <v>49.99</v>
       </c>
       <c r="F43" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1980,10 +2010,10 @@
         <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C44" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D44">
         <v>12</v>
@@ -1992,7 +2022,7 @@
         <v>39.99</v>
       </c>
       <c r="F44" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2000,10 +2030,10 @@
         <v>49</v>
       </c>
       <c r="B45" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C45" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D45">
         <v>11</v>
@@ -2012,7 +2042,7 @@
         <v>49.99</v>
       </c>
       <c r="F45" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2020,10 +2050,10 @@
         <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C46" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D46">
         <v>11</v>
@@ -2032,7 +2062,7 @@
         <v>39.99</v>
       </c>
       <c r="F46" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -2040,10 +2070,10 @@
         <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C47" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D47">
         <v>11</v>
@@ -2052,7 +2082,7 @@
         <v>19.99</v>
       </c>
       <c r="F47" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2060,10 +2090,10 @@
         <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C48" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D48">
         <v>11</v>
@@ -2072,7 +2102,7 @@
         <v>39.99</v>
       </c>
       <c r="F48" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2080,10 +2110,10 @@
         <v>53</v>
       </c>
       <c r="B49" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C49" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D49">
         <v>11</v>
@@ -2092,7 +2122,7 @@
         <v>39.99</v>
       </c>
       <c r="F49" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2100,10 +2130,10 @@
         <v>54</v>
       </c>
       <c r="B50" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C50" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D50">
         <v>11</v>
@@ -2112,7 +2142,7 @@
         <v>49.99</v>
       </c>
       <c r="F50" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2120,10 +2150,10 @@
         <v>55</v>
       </c>
       <c r="B51" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C51" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D51">
         <v>11</v>
@@ -2132,7 +2162,7 @@
         <v>19.99</v>
       </c>
       <c r="F51" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2140,10 +2170,10 @@
         <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C52" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D52">
         <v>11</v>
@@ -2152,7 +2182,7 @@
         <v>39.99</v>
       </c>
       <c r="F52" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2160,10 +2190,10 @@
         <v>57</v>
       </c>
       <c r="B53" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C53" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D53">
         <v>10</v>
@@ -2172,7 +2202,7 @@
         <v>19.99</v>
       </c>
       <c r="F53" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2180,10 +2210,10 @@
         <v>58</v>
       </c>
       <c r="B54" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C54" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D54">
         <v>10</v>
@@ -2192,7 +2222,7 @@
         <v>49.99</v>
       </c>
       <c r="F54" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2200,10 +2230,10 @@
         <v>59</v>
       </c>
       <c r="B55" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C55" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D55">
         <v>10</v>
@@ -2212,7 +2242,7 @@
         <v>39.99</v>
       </c>
       <c r="F55" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2220,10 +2250,10 @@
         <v>60</v>
       </c>
       <c r="B56" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C56" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D56">
         <v>10</v>
@@ -2232,7 +2262,7 @@
         <v>39.99</v>
       </c>
       <c r="F56" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2240,10 +2270,10 @@
         <v>61</v>
       </c>
       <c r="B57" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C57" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D57">
         <v>10</v>
@@ -2252,7 +2282,7 @@
         <v>39.99</v>
       </c>
       <c r="F57" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2260,10 +2290,10 @@
         <v>62</v>
       </c>
       <c r="B58" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C58" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D58">
         <v>10</v>
@@ -2272,7 +2302,7 @@
         <v>19.99</v>
       </c>
       <c r="F58" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2280,10 +2310,10 @@
         <v>63</v>
       </c>
       <c r="B59" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C59" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D59">
         <v>10</v>
@@ -2292,7 +2322,7 @@
         <v>39.99</v>
       </c>
       <c r="F59" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2300,10 +2330,10 @@
         <v>64</v>
       </c>
       <c r="B60" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C60" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D60">
         <v>10</v>
@@ -2312,7 +2342,7 @@
         <v>39.99</v>
       </c>
       <c r="F60" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2320,10 +2350,10 @@
         <v>65</v>
       </c>
       <c r="B61" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C61" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D61">
         <v>10</v>
@@ -2332,7 +2362,7 @@
         <v>49.99</v>
       </c>
       <c r="F61" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2340,10 +2370,10 @@
         <v>66</v>
       </c>
       <c r="B62" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C62" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D62">
         <v>10</v>
@@ -2352,7 +2382,7 @@
         <v>49.99</v>
       </c>
       <c r="F62" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2360,10 +2390,10 @@
         <v>67</v>
       </c>
       <c r="B63" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C63" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D63">
         <v>9</v>
@@ -2372,7 +2402,7 @@
         <v>39.99</v>
       </c>
       <c r="F63" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2380,10 +2410,10 @@
         <v>68</v>
       </c>
       <c r="B64" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C64" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D64">
         <v>9</v>
@@ -2392,7 +2422,7 @@
         <v>19.99</v>
       </c>
       <c r="F64" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2400,10 +2430,10 @@
         <v>69</v>
       </c>
       <c r="B65" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C65" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D65">
         <v>9</v>
@@ -2412,7 +2442,7 @@
         <v>49.99</v>
       </c>
       <c r="F65" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2420,10 +2450,10 @@
         <v>70</v>
       </c>
       <c r="B66" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C66" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D66">
         <v>9</v>
@@ -2432,7 +2462,7 @@
         <v>49.99</v>
       </c>
       <c r="F66" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2440,10 +2470,10 @@
         <v>71</v>
       </c>
       <c r="B67" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C67" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D67">
         <v>9</v>
@@ -2452,7 +2482,7 @@
         <v>19.99</v>
       </c>
       <c r="F67" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2460,10 +2490,10 @@
         <v>72</v>
       </c>
       <c r="B68" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C68" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D68">
         <v>9</v>
@@ -2472,7 +2502,7 @@
         <v>49.99</v>
       </c>
       <c r="F68" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2480,10 +2510,10 @@
         <v>73</v>
       </c>
       <c r="B69" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C69" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D69">
         <v>9</v>
@@ -2492,7 +2522,7 @@
         <v>39.99</v>
       </c>
       <c r="F69" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2500,10 +2530,10 @@
         <v>74</v>
       </c>
       <c r="B70" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C70" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D70">
         <v>9</v>
@@ -2512,7 +2542,7 @@
         <v>19.99</v>
       </c>
       <c r="F70" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2520,10 +2550,10 @@
         <v>75</v>
       </c>
       <c r="B71" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C71" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D71">
         <v>9</v>
@@ -2532,7 +2562,7 @@
         <v>39.99</v>
       </c>
       <c r="F71" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2540,10 +2570,10 @@
         <v>76</v>
       </c>
       <c r="B72" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C72" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D72">
         <v>9</v>
@@ -2552,7 +2582,7 @@
         <v>19.99</v>
       </c>
       <c r="F72" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2560,10 +2590,10 @@
         <v>77</v>
       </c>
       <c r="B73" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C73" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D73">
         <v>9</v>
@@ -2572,7 +2602,7 @@
         <v>49.99</v>
       </c>
       <c r="F73" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2580,10 +2610,10 @@
         <v>78</v>
       </c>
       <c r="B74" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C74" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D74">
         <v>9</v>
@@ -2592,7 +2622,7 @@
         <v>49.99</v>
       </c>
       <c r="F74" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2600,10 +2630,10 @@
         <v>79</v>
       </c>
       <c r="B75" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C75" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D75">
         <v>9</v>
@@ -2612,7 +2642,7 @@
         <v>39.99</v>
       </c>
       <c r="F75" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -2620,10 +2650,10 @@
         <v>80</v>
       </c>
       <c r="B76" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C76" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D76">
         <v>8</v>
@@ -2632,7 +2662,7 @@
         <v>49.99</v>
       </c>
       <c r="F76" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2640,10 +2670,10 @@
         <v>81</v>
       </c>
       <c r="B77" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C77" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D77">
         <v>8</v>
@@ -2652,7 +2682,7 @@
         <v>19.99</v>
       </c>
       <c r="F77" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2660,10 +2690,10 @@
         <v>82</v>
       </c>
       <c r="B78" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C78" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D78">
         <v>8</v>
@@ -2672,7 +2702,7 @@
         <v>49.99</v>
       </c>
       <c r="F78" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2680,10 +2710,10 @@
         <v>83</v>
       </c>
       <c r="B79" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C79" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D79">
         <v>8</v>
@@ -2692,7 +2722,7 @@
         <v>39.99</v>
       </c>
       <c r="F79" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2700,10 +2730,10 @@
         <v>84</v>
       </c>
       <c r="B80" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C80" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="D80">
         <v>8</v>
@@ -2712,7 +2742,7 @@
         <v>39.99</v>
       </c>
       <c r="F80" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2720,10 +2750,10 @@
         <v>85</v>
       </c>
       <c r="B81" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C81" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D81">
         <v>8</v>
@@ -2732,7 +2762,7 @@
         <v>39.99</v>
       </c>
       <c r="F81" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2740,10 +2770,10 @@
         <v>86</v>
       </c>
       <c r="B82" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C82" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D82">
         <v>8</v>
@@ -2752,7 +2782,7 @@
         <v>49.99</v>
       </c>
       <c r="F82" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2760,10 +2790,10 @@
         <v>87</v>
       </c>
       <c r="B83" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C83" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D83">
         <v>8</v>
@@ -2772,7 +2802,7 @@
         <v>49.99</v>
       </c>
       <c r="F83" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2780,10 +2810,10 @@
         <v>88</v>
       </c>
       <c r="B84" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C84" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D84">
         <v>8</v>
@@ -2792,7 +2822,7 @@
         <v>39.99</v>
       </c>
       <c r="F84" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2800,10 +2830,10 @@
         <v>89</v>
       </c>
       <c r="B85" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C85" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D85">
         <v>8</v>
@@ -2812,7 +2842,7 @@
         <v>19.99</v>
       </c>
       <c r="F85" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2820,10 +2850,10 @@
         <v>90</v>
       </c>
       <c r="B86" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C86" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D86">
         <v>8</v>
@@ -2832,7 +2862,7 @@
         <v>39.99</v>
       </c>
       <c r="F86" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2840,10 +2870,10 @@
         <v>91</v>
       </c>
       <c r="B87" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C87" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D87">
         <v>8</v>
@@ -2852,7 +2882,7 @@
         <v>39.99</v>
       </c>
       <c r="F87" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2860,10 +2890,10 @@
         <v>92</v>
       </c>
       <c r="B88" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C88" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D88">
         <v>7</v>
@@ -2872,7 +2902,7 @@
         <v>19.99</v>
       </c>
       <c r="F88" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2880,10 +2910,10 @@
         <v>93</v>
       </c>
       <c r="B89" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C89" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D89">
         <v>7</v>
@@ -2892,7 +2922,7 @@
         <v>39.99</v>
       </c>
       <c r="F89" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -2900,10 +2930,10 @@
         <v>94</v>
       </c>
       <c r="B90" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C90" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="D90">
         <v>7</v>
@@ -2912,7 +2942,7 @@
         <v>39.99</v>
       </c>
       <c r="F90" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -2920,10 +2950,10 @@
         <v>95</v>
       </c>
       <c r="B91" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C91" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D91">
         <v>7</v>
@@ -2932,7 +2962,7 @@
         <v>39.99</v>
       </c>
       <c r="F91" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -2940,10 +2970,10 @@
         <v>96</v>
       </c>
       <c r="B92" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C92" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D92">
         <v>7</v>
@@ -2952,7 +2982,7 @@
         <v>49.99</v>
       </c>
       <c r="F92" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -2960,10 +2990,10 @@
         <v>97</v>
       </c>
       <c r="B93" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C93" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D93">
         <v>7</v>
@@ -2972,7 +3002,7 @@
         <v>49.99</v>
       </c>
       <c r="F93" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -2980,10 +3010,10 @@
         <v>98</v>
       </c>
       <c r="B94" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C94" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D94">
         <v>7</v>
@@ -2992,7 +3022,7 @@
         <v>19.99</v>
       </c>
       <c r="F94" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -3000,10 +3030,10 @@
         <v>99</v>
       </c>
       <c r="B95" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C95" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D95">
         <v>7</v>
@@ -3012,7 +3042,7 @@
         <v>19.99</v>
       </c>
       <c r="F95" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -3020,10 +3050,10 @@
         <v>100</v>
       </c>
       <c r="B96" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C96" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D96">
         <v>7</v>
@@ -3032,7 +3062,7 @@
         <v>19.99</v>
       </c>
       <c r="F96" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -3040,10 +3070,10 @@
         <v>101</v>
       </c>
       <c r="B97" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C97" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D97">
         <v>7</v>
@@ -3052,7 +3082,7 @@
         <v>49.99</v>
       </c>
       <c r="F97" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -3060,10 +3090,10 @@
         <v>102</v>
       </c>
       <c r="B98" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C98" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D98">
         <v>7</v>
@@ -3072,7 +3102,7 @@
         <v>39.99</v>
       </c>
       <c r="F98" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -3080,10 +3110,10 @@
         <v>103</v>
       </c>
       <c r="B99" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C99" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D99">
         <v>7</v>
@@ -3092,7 +3122,7 @@
         <v>49.99</v>
       </c>
       <c r="F99" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -3100,10 +3130,10 @@
         <v>104</v>
       </c>
       <c r="B100" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C100" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D100">
         <v>7</v>
@@ -3112,7 +3142,7 @@
         <v>39.99</v>
       </c>
       <c r="F100" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -3120,10 +3150,10 @@
         <v>105</v>
       </c>
       <c r="B101" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C101" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="D101">
         <v>7</v>
@@ -3132,7 +3162,7 @@
         <v>49.99</v>
       </c>
       <c r="F101" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -3140,10 +3170,10 @@
         <v>106</v>
       </c>
       <c r="B102" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C102" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D102">
         <v>7</v>
@@ -3152,7 +3182,7 @@
         <v>39.99</v>
       </c>
       <c r="F102" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -3160,10 +3190,10 @@
         <v>107</v>
       </c>
       <c r="B103" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C103" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D103">
         <v>7</v>
@@ -3172,7 +3202,7 @@
         <v>49.99</v>
       </c>
       <c r="F103" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -3180,10 +3210,10 @@
         <v>108</v>
       </c>
       <c r="B104" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C104" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D104">
         <v>7</v>
@@ -3192,7 +3222,7 @@
         <v>39.99</v>
       </c>
       <c r="F104" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -3200,10 +3230,10 @@
         <v>109</v>
       </c>
       <c r="B105" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C105" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D105">
         <v>7</v>
@@ -3212,7 +3242,7 @@
         <v>19.99</v>
       </c>
       <c r="F105" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -3220,10 +3250,10 @@
         <v>110</v>
       </c>
       <c r="B106" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C106" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D106">
         <v>7</v>
@@ -3232,7 +3262,7 @@
         <v>19.99</v>
       </c>
       <c r="F106" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -3240,10 +3270,10 @@
         <v>111</v>
       </c>
       <c r="B107" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C107" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D107">
         <v>7</v>
@@ -3252,7 +3282,7 @@
         <v>39.99</v>
       </c>
       <c r="F107" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -3260,10 +3290,10 @@
         <v>112</v>
       </c>
       <c r="B108" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C108" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="D108">
         <v>6</v>
@@ -3272,7 +3302,7 @@
         <v>49.99</v>
       </c>
       <c r="F108" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -3280,10 +3310,10 @@
         <v>113</v>
       </c>
       <c r="B109" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C109" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D109">
         <v>6</v>
@@ -3292,7 +3322,7 @@
         <v>49.99</v>
       </c>
       <c r="F109" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -3300,10 +3330,10 @@
         <v>114</v>
       </c>
       <c r="B110" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C110" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D110">
         <v>6</v>
@@ -3312,7 +3342,7 @@
         <v>39.99</v>
       </c>
       <c r="F110" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -3320,10 +3350,10 @@
         <v>115</v>
       </c>
       <c r="B111" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C111" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D111">
         <v>6</v>
@@ -3332,7 +3362,7 @@
         <v>49.99</v>
       </c>
       <c r="F111" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -3340,10 +3370,10 @@
         <v>116</v>
       </c>
       <c r="B112" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C112" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D112">
         <v>6</v>
@@ -3352,7 +3382,7 @@
         <v>49.99</v>
       </c>
       <c r="F112" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -3360,10 +3390,10 @@
         <v>117</v>
       </c>
       <c r="B113" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C113" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D113">
         <v>6</v>
@@ -3372,7 +3402,7 @@
         <v>39.99</v>
       </c>
       <c r="F113" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -3380,10 +3410,10 @@
         <v>118</v>
       </c>
       <c r="B114" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C114" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D114">
         <v>6</v>
@@ -3392,7 +3422,7 @@
         <v>39.99</v>
       </c>
       <c r="F114" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -3400,10 +3430,10 @@
         <v>119</v>
       </c>
       <c r="B115" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C115" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D115">
         <v>6</v>
@@ -3412,7 +3442,7 @@
         <v>19.99</v>
       </c>
       <c r="F115" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -3420,10 +3450,10 @@
         <v>120</v>
       </c>
       <c r="B116" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C116" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D116">
         <v>6</v>
@@ -3432,7 +3462,7 @@
         <v>39.99</v>
       </c>
       <c r="F116" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -3440,10 +3470,10 @@
         <v>121</v>
       </c>
       <c r="B117" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C117" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D117">
         <v>6</v>
@@ -3452,7 +3482,7 @@
         <v>39.99</v>
       </c>
       <c r="F117" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -3460,10 +3490,10 @@
         <v>122</v>
       </c>
       <c r="B118" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C118" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D118">
         <v>6</v>
@@ -3472,7 +3502,7 @@
         <v>39.99</v>
       </c>
       <c r="F118" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -3480,10 +3510,10 @@
         <v>123</v>
       </c>
       <c r="B119" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C119" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D119">
         <v>6</v>
@@ -3492,7 +3522,7 @@
         <v>39.99</v>
       </c>
       <c r="F119" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -3500,10 +3530,10 @@
         <v>124</v>
       </c>
       <c r="B120" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C120" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D120">
         <v>6</v>
@@ -3512,7 +3542,7 @@
         <v>49.99</v>
       </c>
       <c r="F120" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -3520,10 +3550,10 @@
         <v>125</v>
       </c>
       <c r="B121" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C121" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D121">
         <v>6</v>
@@ -3532,7 +3562,7 @@
         <v>39.99</v>
       </c>
       <c r="F121" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -3540,10 +3570,10 @@
         <v>126</v>
       </c>
       <c r="B122" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C122" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D122">
         <v>6</v>
@@ -3552,7 +3582,7 @@
         <v>39.99</v>
       </c>
       <c r="F122" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -3560,10 +3590,10 @@
         <v>127</v>
       </c>
       <c r="B123" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C123" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D123">
         <v>6</v>
@@ -3572,7 +3602,7 @@
         <v>49.99</v>
       </c>
       <c r="F123" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -3580,10 +3610,10 @@
         <v>128</v>
       </c>
       <c r="B124" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C124" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D124">
         <v>6</v>
@@ -3592,7 +3622,7 @@
         <v>39.99</v>
       </c>
       <c r="F124" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -3600,10 +3630,10 @@
         <v>129</v>
       </c>
       <c r="B125" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C125" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D125">
         <v>6</v>
@@ -3612,7 +3642,7 @@
         <v>49.99</v>
       </c>
       <c r="F125" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -3620,10 +3650,10 @@
         <v>130</v>
       </c>
       <c r="B126" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C126" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D126">
         <v>6</v>
@@ -3632,7 +3662,7 @@
         <v>19.99</v>
       </c>
       <c r="F126" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -3640,10 +3670,10 @@
         <v>131</v>
       </c>
       <c r="B127" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C127" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="D127">
         <v>6</v>
@@ -3652,7 +3682,7 @@
         <v>39.99</v>
       </c>
       <c r="F127" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -3660,10 +3690,10 @@
         <v>132</v>
       </c>
       <c r="B128" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C128" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D128">
         <v>6</v>
@@ -3672,7 +3702,7 @@
         <v>39.99</v>
       </c>
       <c r="F128" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -3680,10 +3710,10 @@
         <v>133</v>
       </c>
       <c r="B129" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C129" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D129">
         <v>6</v>
@@ -3692,7 +3722,7 @@
         <v>39.99</v>
       </c>
       <c r="F129" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -3700,10 +3730,10 @@
         <v>134</v>
       </c>
       <c r="B130" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C130" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D130">
         <v>6</v>
@@ -3712,7 +3742,7 @@
         <v>19.99</v>
       </c>
       <c r="F130" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -3720,10 +3750,10 @@
         <v>135</v>
       </c>
       <c r="B131" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C131" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D131">
         <v>6</v>
@@ -3732,7 +3762,7 @@
         <v>39.99</v>
       </c>
       <c r="F131" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -3740,10 +3770,10 @@
         <v>136</v>
       </c>
       <c r="B132" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C132" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D132">
         <v>6</v>
@@ -3752,7 +3782,7 @@
         <v>39.99</v>
       </c>
       <c r="F132" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="133" spans="1:6">
@@ -3760,10 +3790,10 @@
         <v>137</v>
       </c>
       <c r="B133" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C133" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D133">
         <v>6</v>
@@ -3772,7 +3802,7 @@
         <v>39.99</v>
       </c>
       <c r="F133" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -3780,10 +3810,10 @@
         <v>138</v>
       </c>
       <c r="B134" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C134" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D134">
         <v>6</v>
@@ -3792,7 +3822,7 @@
         <v>19.99</v>
       </c>
       <c r="F134" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
     </row>
     <row r="135" spans="1:6">
@@ -3800,10 +3830,10 @@
         <v>139</v>
       </c>
       <c r="B135" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C135" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D135">
         <v>6</v>
@@ -3812,7 +3842,7 @@
         <v>39.99</v>
       </c>
       <c r="F135" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="136" spans="1:6">
@@ -3820,10 +3850,10 @@
         <v>140</v>
       </c>
       <c r="B136" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C136" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D136">
         <v>6</v>
@@ -3832,7 +3862,7 @@
         <v>19.99</v>
       </c>
       <c r="F136" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
     </row>
     <row r="137" spans="1:6">
@@ -3840,10 +3870,10 @@
         <v>141</v>
       </c>
       <c r="B137" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C137" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D137">
         <v>6</v>
@@ -3852,7 +3882,7 @@
         <v>39.99</v>
       </c>
       <c r="F137" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -3860,10 +3890,10 @@
         <v>142</v>
       </c>
       <c r="B138" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C138" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D138">
         <v>6</v>
@@ -3872,7 +3902,7 @@
         <v>49.99</v>
       </c>
       <c r="F138" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="139" spans="1:6">
@@ -3880,10 +3910,10 @@
         <v>143</v>
       </c>
       <c r="B139" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C139" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D139">
         <v>6</v>
@@ -3892,7 +3922,7 @@
         <v>39.99</v>
       </c>
       <c r="F139" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="140" spans="1:6">
@@ -3900,10 +3930,10 @@
         <v>144</v>
       </c>
       <c r="B140" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C140" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D140">
         <v>6</v>
@@ -3912,7 +3942,7 @@
         <v>39.99</v>
       </c>
       <c r="F140" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
     </row>
     <row r="141" spans="1:6">
@@ -3920,10 +3950,10 @@
         <v>145</v>
       </c>
       <c r="B141" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C141" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D141">
         <v>6</v>
@@ -3932,7 +3962,7 @@
         <v>39.99</v>
       </c>
       <c r="F141" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
     </row>
     <row r="142" spans="1:6">
@@ -3940,10 +3970,10 @@
         <v>146</v>
       </c>
       <c r="B142" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C142" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D142">
         <v>6</v>
@@ -3952,7 +3982,7 @@
         <v>19.99</v>
       </c>
       <c r="F142" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
     </row>
     <row r="143" spans="1:6">
@@ -3960,10 +3990,10 @@
         <v>147</v>
       </c>
       <c r="B143" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C143" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D143">
         <v>5</v>
@@ -3972,7 +4002,7 @@
         <v>49.99</v>
       </c>
       <c r="F143" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
     </row>
     <row r="144" spans="1:6">
@@ -3980,10 +4010,10 @@
         <v>148</v>
       </c>
       <c r="B144" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C144" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D144">
         <v>5</v>
@@ -3992,7 +4022,7 @@
         <v>39.99</v>
       </c>
       <c r="F144" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="145" spans="1:6">
@@ -4000,10 +4030,10 @@
         <v>149</v>
       </c>
       <c r="B145" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C145" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D145">
         <v>5</v>
@@ -4012,7 +4042,7 @@
         <v>39.99</v>
       </c>
       <c r="F145" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="146" spans="1:6">
@@ -4020,10 +4050,10 @@
         <v>150</v>
       </c>
       <c r="B146" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C146" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D146">
         <v>5</v>
@@ -4032,7 +4062,7 @@
         <v>39.99</v>
       </c>
       <c r="F146" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="147" spans="1:6">
@@ -4040,10 +4070,10 @@
         <v>151</v>
       </c>
       <c r="B147" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C147" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D147">
         <v>5</v>
@@ -4052,7 +4082,7 @@
         <v>39.99</v>
       </c>
       <c r="F147" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
     </row>
     <row r="148" spans="1:6">
@@ -4060,10 +4090,10 @@
         <v>152</v>
       </c>
       <c r="B148" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C148" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D148">
         <v>5</v>
@@ -4072,7 +4102,7 @@
         <v>19.99</v>
       </c>
       <c r="F148" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="149" spans="1:6">
@@ -4080,10 +4110,10 @@
         <v>153</v>
       </c>
       <c r="B149" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C149" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D149">
         <v>5</v>
@@ -4092,7 +4122,7 @@
         <v>19.99</v>
       </c>
       <c r="F149" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="150" spans="1:6">
@@ -4100,10 +4130,10 @@
         <v>154</v>
       </c>
       <c r="B150" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C150" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D150">
         <v>5</v>
@@ -4112,7 +4142,7 @@
         <v>39.99</v>
       </c>
       <c r="F150" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
     </row>
     <row r="151" spans="1:6">
@@ -4120,10 +4150,10 @@
         <v>155</v>
       </c>
       <c r="B151" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C151" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D151">
         <v>5</v>
@@ -4132,7 +4162,7 @@
         <v>49.99</v>
       </c>
       <c r="F151" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="152" spans="1:6">
@@ -4140,10 +4170,10 @@
         <v>156</v>
       </c>
       <c r="B152" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C152" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D152">
         <v>5</v>
@@ -4152,7 +4182,7 @@
         <v>19.99</v>
       </c>
       <c r="F152" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="153" spans="1:6">
@@ -4160,10 +4190,10 @@
         <v>157</v>
       </c>
       <c r="B153" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C153" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D153">
         <v>5</v>
@@ -4172,7 +4202,7 @@
         <v>19.99</v>
       </c>
       <c r="F153" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="154" spans="1:6">
@@ -4180,10 +4210,10 @@
         <v>158</v>
       </c>
       <c r="B154" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C154" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D154">
         <v>5</v>
@@ -4192,7 +4222,7 @@
         <v>49.99</v>
       </c>
       <c r="F154" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
     </row>
     <row r="155" spans="1:6">
@@ -4200,10 +4230,10 @@
         <v>159</v>
       </c>
       <c r="B155" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C155" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D155">
         <v>5</v>
@@ -4212,7 +4242,7 @@
         <v>39.99</v>
       </c>
       <c r="F155" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="156" spans="1:6">
@@ -4220,10 +4250,10 @@
         <v>160</v>
       </c>
       <c r="B156" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C156" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="D156">
         <v>5</v>
@@ -4232,7 +4262,7 @@
         <v>39.99</v>
       </c>
       <c r="F156" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
     </row>
     <row r="157" spans="1:6">
@@ -4240,10 +4270,10 @@
         <v>161</v>
       </c>
       <c r="B157" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C157" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D157">
         <v>5</v>
@@ -4252,7 +4282,7 @@
         <v>39.99</v>
       </c>
       <c r="F157" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="158" spans="1:6">
@@ -4260,10 +4290,10 @@
         <v>162</v>
       </c>
       <c r="B158" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C158" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D158">
         <v>5</v>
@@ -4272,7 +4302,7 @@
         <v>39.99</v>
       </c>
       <c r="F158" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="159" spans="1:6">
@@ -4280,10 +4310,10 @@
         <v>163</v>
       </c>
       <c r="B159" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C159" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D159">
         <v>5</v>
@@ -4292,7 +4322,7 @@
         <v>39.99</v>
       </c>
       <c r="F159" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="160" spans="1:6">
@@ -4300,10 +4330,10 @@
         <v>164</v>
       </c>
       <c r="B160" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C160" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D160">
         <v>5</v>
@@ -4312,7 +4342,7 @@
         <v>19.99</v>
       </c>
       <c r="F160" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="161" spans="1:6">
@@ -4320,10 +4350,10 @@
         <v>165</v>
       </c>
       <c r="B161" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C161" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D161">
         <v>5</v>
@@ -4332,7 +4362,7 @@
         <v>39.99</v>
       </c>
       <c r="F161" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="162" spans="1:6">
@@ -4340,10 +4370,10 @@
         <v>166</v>
       </c>
       <c r="B162" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C162" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D162">
         <v>5</v>
@@ -4352,7 +4382,7 @@
         <v>39.99</v>
       </c>
       <c r="F162" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
     </row>
     <row r="163" spans="1:6">
@@ -4360,10 +4390,10 @@
         <v>167</v>
       </c>
       <c r="B163" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C163" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D163">
         <v>5</v>
@@ -4372,7 +4402,7 @@
         <v>49.99</v>
       </c>
       <c r="F163" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="164" spans="1:6">
@@ -4380,10 +4410,10 @@
         <v>168</v>
       </c>
       <c r="B164" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C164" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D164">
         <v>5</v>
@@ -4392,7 +4422,7 @@
         <v>39.99</v>
       </c>
       <c r="F164" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="165" spans="1:6">
@@ -4400,10 +4430,10 @@
         <v>169</v>
       </c>
       <c r="B165" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C165" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D165">
         <v>5</v>
@@ -4412,7 +4442,7 @@
         <v>19.99</v>
       </c>
       <c r="F165" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="166" spans="1:6">
@@ -4420,10 +4450,10 @@
         <v>170</v>
       </c>
       <c r="B166" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C166" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D166">
         <v>5</v>
@@ -4432,7 +4462,7 @@
         <v>19.99</v>
       </c>
       <c r="F166" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="167" spans="1:6">
@@ -4440,10 +4470,10 @@
         <v>171</v>
       </c>
       <c r="B167" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C167" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D167">
         <v>5</v>
@@ -4452,7 +4482,7 @@
         <v>19.99</v>
       </c>
       <c r="F167" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
     </row>
     <row r="168" spans="1:6">
@@ -4460,10 +4490,10 @@
         <v>172</v>
       </c>
       <c r="B168" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C168" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D168">
         <v>5</v>
@@ -4472,7 +4502,7 @@
         <v>39.99</v>
       </c>
       <c r="F168" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="169" spans="1:6">
@@ -4480,10 +4510,10 @@
         <v>173</v>
       </c>
       <c r="B169" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C169" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D169">
         <v>5</v>
@@ -4492,7 +4522,7 @@
         <v>19.99</v>
       </c>
       <c r="F169" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="170" spans="1:6">
@@ -4500,10 +4530,10 @@
         <v>174</v>
       </c>
       <c r="B170" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C170" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D170">
         <v>5</v>
@@ -4512,7 +4542,7 @@
         <v>39.99</v>
       </c>
       <c r="F170" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="171" spans="1:6">
@@ -4520,10 +4550,10 @@
         <v>175</v>
       </c>
       <c r="B171" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C171" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D171">
         <v>5</v>
@@ -4532,7 +4562,7 @@
         <v>19.99</v>
       </c>
       <c r="F171" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
     </row>
     <row r="172" spans="1:6">
@@ -4540,10 +4570,10 @@
         <v>176</v>
       </c>
       <c r="B172" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C172" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D172">
         <v>5</v>
@@ -4552,7 +4582,7 @@
         <v>59.99</v>
       </c>
       <c r="F172" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="173" spans="1:6">
@@ -4560,10 +4590,10 @@
         <v>177</v>
       </c>
       <c r="B173" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C173" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D173">
         <v>5</v>
@@ -4572,7 +4602,7 @@
         <v>39.99</v>
       </c>
       <c r="F173" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="174" spans="1:6">
@@ -4580,10 +4610,10 @@
         <v>178</v>
       </c>
       <c r="B174" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C174" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D174">
         <v>5</v>
@@ -4592,7 +4622,7 @@
         <v>49.99</v>
       </c>
       <c r="F174" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="175" spans="1:6">
@@ -4600,10 +4630,10 @@
         <v>179</v>
       </c>
       <c r="B175" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C175" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D175">
         <v>5</v>
@@ -4612,7 +4642,7 @@
         <v>39.99</v>
       </c>
       <c r="F175" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="176" spans="1:6">
@@ -4620,10 +4650,10 @@
         <v>180</v>
       </c>
       <c r="B176" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C176" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="D176">
         <v>5</v>
@@ -4632,7 +4662,7 @@
         <v>49.99</v>
       </c>
       <c r="F176" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="177" spans="1:6">
@@ -4640,10 +4670,10 @@
         <v>181</v>
       </c>
       <c r="B177" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C177" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D177">
         <v>5</v>
@@ -4652,7 +4682,7 @@
         <v>19.99</v>
       </c>
       <c r="F177" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="178" spans="1:6">
@@ -4660,10 +4690,10 @@
         <v>182</v>
       </c>
       <c r="B178" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C178" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D178">
         <v>5</v>
@@ -4672,7 +4702,7 @@
         <v>49.99</v>
       </c>
       <c r="F178" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="179" spans="1:6">
@@ -4680,10 +4710,10 @@
         <v>183</v>
       </c>
       <c r="B179" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C179" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D179">
         <v>5</v>
@@ -4692,7 +4722,7 @@
         <v>39.99</v>
       </c>
       <c r="F179" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="180" spans="1:6">
@@ -4700,10 +4730,10 @@
         <v>184</v>
       </c>
       <c r="B180" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C180" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D180">
         <v>5</v>
@@ -4712,7 +4742,7 @@
         <v>49.99</v>
       </c>
       <c r="F180" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="181" spans="1:6">
@@ -4720,10 +4750,10 @@
         <v>185</v>
       </c>
       <c r="B181" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C181" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D181">
         <v>5</v>
@@ -4732,7 +4762,7 @@
         <v>39.99</v>
       </c>
       <c r="F181" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
     </row>
     <row r="182" spans="1:6">
@@ -4740,10 +4770,10 @@
         <v>186</v>
       </c>
       <c r="B182" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C182" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D182">
         <v>5</v>
@@ -4752,7 +4782,7 @@
         <v>39.99</v>
       </c>
       <c r="F182" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="183" spans="1:6">
@@ -4760,10 +4790,10 @@
         <v>187</v>
       </c>
       <c r="B183" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C183" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D183">
         <v>5</v>
@@ -4772,7 +4802,7 @@
         <v>39.99</v>
       </c>
       <c r="F183" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="184" spans="1:6">
@@ -4780,10 +4810,10 @@
         <v>188</v>
       </c>
       <c r="B184" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C184" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="D184">
         <v>5</v>
@@ -4792,7 +4822,7 @@
         <v>49.99</v>
       </c>
       <c r="F184" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="185" spans="1:6">
@@ -4800,10 +4830,10 @@
         <v>189</v>
       </c>
       <c r="B185" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C185" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D185">
         <v>5</v>
@@ -4812,7 +4842,7 @@
         <v>19.99</v>
       </c>
       <c r="F185" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="186" spans="1:6">
@@ -4820,10 +4850,10 @@
         <v>190</v>
       </c>
       <c r="B186" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C186" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D186">
         <v>5</v>
@@ -4832,7 +4862,7 @@
         <v>39.99</v>
       </c>
       <c r="F186" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
     </row>
     <row r="187" spans="1:6">
@@ -4840,10 +4870,10 @@
         <v>191</v>
       </c>
       <c r="B187" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C187" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D187">
         <v>5</v>
@@ -4852,7 +4882,7 @@
         <v>39.99</v>
       </c>
       <c r="F187" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
     </row>
     <row r="188" spans="1:6">
@@ -4860,10 +4890,10 @@
         <v>192</v>
       </c>
       <c r="B188" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C188" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="D188">
         <v>5</v>
@@ -4872,7 +4902,7 @@
         <v>49.99</v>
       </c>
       <c r="F188" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="189" spans="1:6">
@@ -4880,10 +4910,10 @@
         <v>193</v>
       </c>
       <c r="B189" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C189" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="D189">
         <v>5</v>
@@ -4892,7 +4922,7 @@
         <v>39.99</v>
       </c>
       <c r="F189" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="190" spans="1:6">
@@ -4900,10 +4930,10 @@
         <v>194</v>
       </c>
       <c r="B190" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C190" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D190">
         <v>5</v>
@@ -4912,7 +4942,7 @@
         <v>39.99</v>
       </c>
       <c r="F190" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="191" spans="1:6">
@@ -4920,10 +4950,10 @@
         <v>195</v>
       </c>
       <c r="B191" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C191" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D191">
         <v>5</v>
@@ -4932,7 +4962,7 @@
         <v>19.99</v>
       </c>
       <c r="F191" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="192" spans="1:6">
@@ -4940,19 +4970,19 @@
         <v>196</v>
       </c>
       <c r="B192" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C192" t="s">
-        <v>210</v>
+        <v>227</v>
       </c>
       <c r="D192">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="E192">
-        <v>49.99</v>
+        <v>40</v>
       </c>
       <c r="F192" t="s">
-        <v>227</v>
+        <v>252</v>
       </c>
     </row>
     <row r="193" spans="1:6">
@@ -4960,19 +4990,19 @@
         <v>197</v>
       </c>
       <c r="B193" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C193" t="s">
-        <v>210</v>
+        <v>227</v>
       </c>
       <c r="D193">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="E193">
-        <v>49.99</v>
+        <v>40</v>
       </c>
       <c r="F193" t="s">
-        <v>229</v>
+        <v>252</v>
       </c>
     </row>
     <row r="194" spans="1:6">
@@ -4980,19 +5010,19 @@
         <v>198</v>
       </c>
       <c r="B194" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C194" t="s">
-        <v>210</v>
+        <v>227</v>
       </c>
       <c r="D194">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E194">
-        <v>39.99</v>
+        <v>40</v>
       </c>
       <c r="F194" t="s">
-        <v>229</v>
+        <v>252</v>
       </c>
     </row>
     <row r="195" spans="1:6">
@@ -5000,19 +5030,19 @@
         <v>199</v>
       </c>
       <c r="B195" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C195" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="D195">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E195">
-        <v>39.99</v>
+        <v>40</v>
       </c>
       <c r="F195" t="s">
-        <v>229</v>
+        <v>252</v>
       </c>
     </row>
     <row r="196" spans="1:6">
@@ -5020,19 +5050,19 @@
         <v>200</v>
       </c>
       <c r="B196" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C196" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="D196">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="E196">
-        <v>49.99</v>
+        <v>40</v>
       </c>
       <c r="F196" t="s">
-        <v>229</v>
+        <v>252</v>
       </c>
     </row>
     <row r="197" spans="1:6">
@@ -5040,19 +5070,19 @@
         <v>201</v>
       </c>
       <c r="B197" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C197" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="D197">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="E197">
-        <v>39.99</v>
+        <v>60</v>
       </c>
       <c r="F197" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
     </row>
     <row r="198" spans="1:6">
@@ -5060,19 +5090,19 @@
         <v>202</v>
       </c>
       <c r="B198" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C198" t="s">
-        <v>212</v>
+        <v>227</v>
       </c>
       <c r="D198">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="E198">
-        <v>19.99</v>
+        <v>60</v>
       </c>
       <c r="F198" t="s">
-        <v>224</v>
+        <v>253</v>
       </c>
     </row>
     <row r="199" spans="1:6">
@@ -5080,19 +5110,59 @@
         <v>203</v>
       </c>
       <c r="B199" t="s">
+        <v>207</v>
+      </c>
+      <c r="C199" t="s">
+        <v>228</v>
+      </c>
+      <c r="D199">
+        <v>44</v>
+      </c>
+      <c r="E199">
+        <v>30</v>
+      </c>
+      <c r="F199" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6">
+      <c r="A200" t="s">
         <v>204</v>
       </c>
-      <c r="C199" t="s">
-        <v>207</v>
-      </c>
-      <c r="D199">
-        <v>5</v>
-      </c>
-      <c r="E199">
-        <v>19.99</v>
-      </c>
-      <c r="F199" t="s">
-        <v>224</v>
+      <c r="B200" t="s">
+        <v>207</v>
+      </c>
+      <c r="C200" t="s">
+        <v>229</v>
+      </c>
+      <c r="D200">
+        <v>99</v>
+      </c>
+      <c r="E200">
+        <v>100</v>
+      </c>
+      <c r="F200" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6">
+      <c r="A201" t="s">
+        <v>205</v>
+      </c>
+      <c r="B201" t="s">
+        <v>207</v>
+      </c>
+      <c r="C201" t="s">
+        <v>229</v>
+      </c>
+      <c r="D201">
+        <v>99</v>
+      </c>
+      <c r="E201">
+        <v>100</v>
+      </c>
+      <c r="F201" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>